<commit_message>
:sparkles: feat: Adicionando os dados pré calculados no XLSX
</commit_message>
<xml_diff>
--- a/API/src/app/predictionModel/Dados.xlsx
+++ b/API/src/app/predictionModel/Dados.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>índice</t>
   </si>
@@ -87,12 +87,6 @@
   </si>
   <si>
     <t>Cascavel</t>
-  </si>
-  <si>
-    <t>13/05/2021</t>
-  </si>
-  <si>
-    <t>19/05/2021</t>
   </si>
   <si>
     <t>tamanho da previsão (em dias)</t>
@@ -348,42 +342,35 @@
       <c r="I2">
         <v>31826</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>24</v>
+      <c r="J2" s="1">
+        <v>44329</v>
       </c>
       <c r="K2">
-        <f>C2-D2</f>
-        <v>285402</v>
+        <v>298930</v>
       </c>
       <c r="L2">
-        <f>D2-E2-F2</f>
-        <v>1509</v>
+        <v>1455</v>
       </c>
       <c r="M2">
-        <f>E2+F2</f>
-        <v>7249</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>31948</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44335</v>
       </c>
       <c r="O2">
-        <f>C2-G2</f>
-        <v>284991</v>
+        <v>298343</v>
       </c>
       <c r="P2">
-        <f>G2-H2-I2</f>
-        <v>1743</v>
+        <v>1476</v>
       </c>
       <c r="Q2">
-        <f>H2+I2</f>
-        <v>7426</v>
+        <v>32514</v>
       </c>
       <c r="R2">
         <v>6</v>
       </c>
       <c r="S2" s="2">
-        <f>H2/Q2</f>
-        <v>0.0269323996768112</v>
+        <v>0.021160115642492466</v>
       </c>
       <c r="T2" s="3">
         <v>0.35</v>
@@ -572,7 +559,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1">
         <v>30</v>
@@ -580,7 +567,7 @@
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4">
         <f>COUNT(sir!A:A)</f>
@@ -589,7 +576,7 @@
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>0.08</v>
@@ -597,7 +584,7 @@
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>0.05</v>
@@ -605,7 +592,7 @@
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -613,7 +600,7 @@
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>0.001</v>
@@ -621,7 +608,7 @@
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>14</v>

</xml_diff>